<commit_message>
Script gui permettant de créer des chemins ou des trous. Prochaine étape: chemins en 3d
</commit_message>
<xml_diff>
--- a/eg/trous.xlsx
+++ b/eg/trous.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Émile Jetzer\polymtl.ca\Techniciens Génie Physique - Documents\Projets en cours\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilejetzer/Documents/Polytechnique/Répertoires de code/assistant-charlygraal/eg/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{0A102C18-ACC3-E44F-8FF3-6855D585CA0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16695" windowHeight="12120"/>
+    <workbookView xWindow="15940" yWindow="2680" windowWidth="22300" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -171,8 +172,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,8 +239,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{3F26BF96-D435-40C7-85B1-0FC3A957714A}">
-  <header guid="{3F26BF96-D435-40C7-85B1-0FC3A957714A}" dateTime="2021-10-13T11:18:25" maxSheetId="2" userName="Émile Jetzer" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{9FED6C59-161E-3641-A9D1-C11F0281D616}" diskRevisions="1" revisionId="50" version="2">
+  <header guid="{9FED6C59-161E-3641-A9D1-C11F0281D616}" dateTime="2022-07-11T15:49:36" maxSheetId="2" userName="Émile Jetzer" r:id="rId2" minRId="1" maxRId="50">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -247,8 +248,251 @@
 </headers>
 </file>
 
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="1" sId="1" ref="D1:D1048576" action="insertCol"/>
+  <rrc rId="2" sId="1" ref="E1:E1048576" action="insertCol"/>
+  <rcc rId="3" sId="1">
+    <nc r="D2">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="4" sId="1">
+    <nc r="E2">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="5" sId="1">
+    <nc r="D3">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="6" sId="1">
+    <nc r="E3">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="7" sId="1">
+    <nc r="D4">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="8" sId="1">
+    <nc r="E4">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="9" sId="1">
+    <nc r="D5">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="10" sId="1">
+    <nc r="E5">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="11" sId="1">
+    <nc r="D6">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="12" sId="1">
+    <nc r="E6">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="13" sId="1">
+    <nc r="D7">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="14" sId="1">
+    <nc r="E7">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="15" sId="1">
+    <nc r="D8">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="16" sId="1">
+    <nc r="E8">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="17" sId="1">
+    <nc r="D9">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="18" sId="1">
+    <nc r="E9">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="19" sId="1">
+    <nc r="D10">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="20" sId="1">
+    <nc r="E10">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="21" sId="1">
+    <nc r="D11">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="22" sId="1">
+    <nc r="E11">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="23" sId="1">
+    <nc r="D12">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="24" sId="1">
+    <nc r="E12">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="25" sId="1">
+    <nc r="D13">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="26" sId="1">
+    <nc r="E13">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="27" sId="1">
+    <nc r="D14">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="28" sId="1">
+    <nc r="E14">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="29" sId="1">
+    <nc r="D15">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="30" sId="1">
+    <nc r="E15">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="31" sId="1">
+    <nc r="D16">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="32" sId="1">
+    <nc r="E16">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="33" sId="1">
+    <nc r="D17">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="34" sId="1">
+    <nc r="E17">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="35" sId="1">
+    <nc r="D18">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="36" sId="1">
+    <nc r="E18">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="37" sId="1">
+    <nc r="D19">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="38" sId="1">
+    <nc r="E19">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="39" sId="1">
+    <nc r="D20">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="40" sId="1">
+    <nc r="E20">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="41" sId="1">
+    <nc r="D21">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="42" sId="1">
+    <nc r="E21">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="43" sId="1">
+    <nc r="D22">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="44" sId="1">
+    <nc r="E22">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="45" sId="1">
+    <nc r="D23">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="46" sId="1">
+    <nc r="E23">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="47" sId="1">
+    <nc r="D24">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="48" sId="1">
+    <nc r="E24">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="49" sId="1">
+    <nc r="D25">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="50" sId="1">
+    <nc r="E25">
+      <v>11</v>
+    </nc>
+  </rcc>
+</revisions>
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
@@ -517,19 +761,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="46">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,11 +786,13 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="23">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -553,11 +802,17 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="23">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -567,11 +822,17 @@
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="23">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -581,11 +842,17 @@
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="23">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -595,11 +862,17 @@
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="23">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -609,11 +882,17 @@
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="23">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -623,11 +902,17 @@
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1">
+        <v>11</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="23">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -637,11 +922,17 @@
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="23">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -651,11 +942,17 @@
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1">
+        <v>11</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="23">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -665,11 +962,17 @@
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1">
+        <v>11</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="23">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -679,11 +982,17 @@
       <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1">
+        <v>11</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="23">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -693,11 +1002,17 @@
       <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1">
+        <v>11</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="23">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -707,11 +1022,17 @@
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1">
+        <v>11</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="23">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -721,11 +1042,17 @@
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1">
+        <v>11</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="23">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -735,11 +1062,17 @@
       <c r="C15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1">
+        <v>11</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="23">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -749,11 +1082,17 @@
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1">
+        <v>11</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="23">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -763,11 +1102,17 @@
       <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1">
+        <v>11</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="23">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -777,11 +1122,17 @@
       <c r="C18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1">
+        <v>11</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="23">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -791,11 +1142,17 @@
       <c r="C19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1">
+        <v>11</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="23">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -805,11 +1162,17 @@
       <c r="C20" s="1">
         <v>-12</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1">
+        <v>11</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="23">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -819,11 +1182,17 @@
       <c r="C21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1">
+        <v>10</v>
+      </c>
+      <c r="E21" s="1">
+        <v>11</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="23">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -833,11 +1202,17 @@
       <c r="C22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1">
+        <v>11</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="23">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -847,11 +1222,17 @@
       <c r="C23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1">
+        <v>11</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="23">
       <c r="A24" s="1" t="s">
         <v>37</v>
       </c>
@@ -861,11 +1242,17 @@
       <c r="C24" s="1">
         <v>-293</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1">
+        <v>11</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="23">
       <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
@@ -875,7 +1262,13 @@
       <c r="C25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="1">
+        <v>10</v>
+      </c>
+      <c r="E25" s="1">
+        <v>11</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -892,6 +1285,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100447C80396883E44C97F93366B537FD40" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="cce9e7eabd10cecda661398d47fd0271">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3e7a6ef-71bd-4131-9933-e0e605c48bb6" xmlns:ns3="cb3cc569-0727-44bc-a837-5afadc187092" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="102afac0f6f37dac49fc788080ce3a40" ns2:_="" ns3:_="">
     <xsd:import namespace="d3e7a6ef-71bd-4131-9933-e0e605c48bb6"/>
@@ -1114,29 +1522,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2748BAE-126A-4F6A-AD5E-4F55750A4968}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5368F19F-DE46-4385-8595-0B774311633A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F73F3E3-5935-4325-B0A2-04513E413B0B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F73F3E3-5935-4325-B0A2-04513E413B0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5368F19F-DE46-4385-8595-0B774311633A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2748BAE-126A-4F6A-AD5E-4F55750A4968}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d3e7a6ef-71bd-4131-9933-e0e605c48bb6"/>
+    <ds:schemaRef ds:uri="cb3cc569-0727-44bc-a837-5afadc187092"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>